<commit_message>
add some modified files
</commit_message>
<xml_diff>
--- a/docs/uec_iot_esc_sounds_list.xlsx
+++ b/docs/uec_iot_esc_sounds_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20405"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xrickliao/WorkSpaces/Work/Projects/TransferLearning_for_ACDNet/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Prjects\TransferLearning_for_ACDNet\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6BC6095D-D56A-6842-9E0A-E692AAD7B7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAD8C91-E2AF-41C6-A642-AB4190A42CF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21820" xr2:uid="{16796A70-B98A-E545-9E50-4B02BC7D9A33}"/>
+    <workbookView xWindow="0" yWindow="504" windowWidth="38400" windowHeight="21816" xr2:uid="{16796A70-B98A-E545-9E50-4B02BC7D9A33}"/>
   </bookViews>
   <sheets>
     <sheet name="sounds-meta-data" sheetId="1" r:id="rId1"/>
@@ -21,22 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>sound file name(name-tag.wav(mp3))</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -74,14 +64,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>fire-alarm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Line-App-Official-Ring-Sounds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>shower-water</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -99,6 +81,50 @@
   </si>
   <si>
     <t>num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alarm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All alert sounds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ringtone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Line and WeChat default</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pain-sound</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foot-setp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>not-need now</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>first-sage included</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*:表示用更多聲音進行訓練</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>熱水壺笛聲</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -106,7 +132,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -124,6 +150,14 @@
     </font>
     <font>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="新細明體"/>
       <family val="2"/>
@@ -168,11 +202,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -489,23 +526,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A99354B-A373-0142-8D61-54B41A18C11C}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="29.1640625" defaultRowHeight="25"/>
+  <sheetFormatPr defaultColWidth="29.109375" defaultRowHeight="24.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="29.1640625" style="1"/>
-    <col min="3" max="3" width="43.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.33203125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="29.1640625" style="1"/>
+    <col min="1" max="1" width="17.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" style="1"/>
+    <col min="6" max="6" width="41.88671875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="29.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -516,8 +556,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -528,7 +571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -538,8 +581,14 @@
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -549,8 +598,11 @@
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -560,8 +612,14 @@
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -569,10 +627,16 @@
         <v>52</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -583,7 +647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -591,10 +655,13 @@
         <v>54</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -602,10 +669,10 @@
         <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -613,34 +680,60 @@
         <v>56</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>98</v>
+        <v>57</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1">
+        <v>58</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>98</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
         <v>99</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>14</v>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -652,19 +745,19 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="29.1640625" defaultRowHeight="25"/>
+  <sheetFormatPr defaultColWidth="29.109375" defaultRowHeight="24.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" style="1"/>
-    <col min="2" max="2" width="50.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.1640625" style="1"/>
-    <col min="4" max="4" width="43.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" style="1"/>
+    <col min="2" max="2" width="50.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" style="1"/>
+    <col min="4" max="4" width="43.77734375" style="1" customWidth="1"/>
     <col min="5" max="5" width="38.33203125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="29.1640625" style="1"/>
+    <col min="6" max="16384" width="29.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -679,57 +772,57 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
modify some data and folder name
</commit_message>
<xml_diff>
--- a/docs/uec_iot_esc_sounds_list.xlsx
+++ b/docs/uec_iot_esc_sounds_list.xlsx
@@ -50,6 +50,12 @@
     <t xml:space="preserve">*:表示用更多聲音進行訓練</t>
   </si>
   <si>
+    <t xml:space="preserve">sneezing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not-need now</t>
+  </si>
+  <si>
     <t xml:space="preserve">coughing</t>
   </si>
   <si>
@@ -75,12 +81,6 @@
   </si>
   <si>
     <t xml:space="preserve">shower-water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sneezing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not-need now</t>
   </si>
   <si>
     <t xml:space="preserve">pain-sound</t>
@@ -222,10 +222,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.09765625" defaultRowHeight="24" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -284,31 +284,29 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -317,10 +315,10 @@
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -334,57 +332,60 @@
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="D9" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
         <v>9</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
-        <v>10</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>57</v>
@@ -392,10 +393,11 @@
       <c r="C11" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>58</v>
@@ -404,9 +406,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>98</v>
@@ -415,9 +417,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>99</v>
@@ -425,6 +427,13 @@
       <c r="C14" s="1" t="s">
         <v>23</v>
       </c>
+    </row>
+    <row r="15" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>